<commit_message>
Search Portal WoW: add blank row above WoW section
</commit_message>
<xml_diff>
--- a/3/DAGenerators/Spreadsheets/Templates/search/SearchPPCtemplate.xlsx
+++ b/3/DAGenerators/Spreadsheets/Templates/search/SearchPPCtemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DA\portal\search\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\da-projects\3\DAGenerators\Spreadsheets\Templates\search\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="255" windowWidth="20055" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9705"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="41">
   <si>
     <t>Clicks</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>Search Campaigns</t>
+  </si>
+  <si>
+    <t>WoW Summary</t>
+  </si>
+  <si>
+    <t>WoW Change</t>
   </si>
 </sst>
 </file>
@@ -797,9 +803,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B8:T53"/>
+  <dimension ref="B8:T60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1284,471 +1292,690 @@
     </row>
     <row r="23" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="13"/>
-    </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B24" s="43" t="s">
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+    </row>
+    <row r="24" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="B24" s="7"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="13"/>
+    </row>
+    <row r="25" spans="2:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="R26" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="B27" s="7"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="15">
+        <f>IFERROR(C27/D27,)</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="16"/>
+      <c r="G27" s="14">
+        <f>IFERROR(F27/C27,)</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="17"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14">
+        <f>I27-F27</f>
+        <v>0</v>
+      </c>
+      <c r="K27" s="17"/>
+      <c r="L27" s="14" t="str">
+        <f>IF(K27&gt;0,K27*20,"-")</f>
+        <v>-</v>
+      </c>
+      <c r="M27" s="17"/>
+      <c r="N27" s="34"/>
+      <c r="O27" s="14">
+        <f>IFERROR(F27/H27,)</f>
+        <v>0</v>
+      </c>
+      <c r="P27" s="15">
+        <f>IFERROR(H27/C27,)</f>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="14">
+        <f>IFERROR(I27/H27,)</f>
+        <v>0</v>
+      </c>
+      <c r="R27" s="13">
+        <f>IFERROR(I27/F27,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="15">
+        <f>IFERROR(C28/D28,)</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="16"/>
+      <c r="G28" s="14">
+        <f>IFERROR(F28/C28,)</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="17"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14">
+        <f>I28-F28</f>
+        <v>0</v>
+      </c>
+      <c r="K28" s="17"/>
+      <c r="L28" s="14" t="str">
+        <f>IF(K28&gt;0,K28*20,"-")</f>
+        <v>-</v>
+      </c>
+      <c r="M28" s="17"/>
+      <c r="N28" s="34"/>
+      <c r="O28" s="14">
+        <f>IFERROR(F28/H28,)</f>
+        <v>0</v>
+      </c>
+      <c r="P28" s="15">
+        <f>IFERROR(H28/C28,)</f>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="14">
+        <f>IFERROR(I28/H28,)</f>
+        <v>0</v>
+      </c>
+      <c r="R28" s="13">
+        <f>IFERROR(I28/F28,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="B29" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+    </row>
+    <row r="30" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="B30" s="7"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="13"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="43"/>
-      <c r="O24" s="43"/>
-      <c r="P24" s="43"/>
-      <c r="Q24" s="43"/>
-      <c r="R24" s="43"/>
-      <c r="S24" s="43"/>
-      <c r="T24" s="43"/>
-    </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="O28" s="8"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
-    </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B43" s="10" t="s">
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="43"/>
+      <c r="L31" s="43"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="43"/>
+      <c r="O31" s="43"/>
+      <c r="P31" s="43"/>
+      <c r="Q31" s="43"/>
+      <c r="R31" s="43"/>
+      <c r="S31" s="43"/>
+      <c r="T31" s="43"/>
+    </row>
+    <row r="35" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O35" s="8"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
+    </row>
+    <row r="50" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B50" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
-      <c r="O43" s="2"/>
-      <c r="P43" s="2"/>
-      <c r="Q43" s="2"/>
-      <c r="R43" s="2"/>
-      <c r="S43" s="2"/>
-      <c r="T43" s="2"/>
-    </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2"/>
+      <c r="S50" s="2"/>
+      <c r="T50" s="2"/>
+    </row>
+    <row r="51" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D44" s="4" t="s">
+      <c r="C51" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E51" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F51" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G44" s="5" t="s">
+      <c r="G51" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H44" s="4" t="s">
+      <c r="H51" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I44" s="4" t="s">
+      <c r="I51" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J44" s="4" t="s">
+      <c r="J51" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K44" s="4" t="s">
+      <c r="K51" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L44" s="4" t="s">
+      <c r="L51" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M44" s="4" t="s">
+      <c r="M51" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="N44" s="4" t="s">
+      <c r="N51" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="O44" s="4" t="s">
+      <c r="O51" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P44" s="6" t="s">
+      <c r="P51" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q44" s="4" t="s">
+      <c r="Q51" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="R44" s="6" t="s">
+      <c r="R51" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="B45" s="18"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="15">
-        <f t="shared" ref="E45" si="0">IFERROR(C45/D45,)</f>
-        <v>0</v>
-      </c>
-      <c r="F45" s="16"/>
-      <c r="G45" s="14">
-        <f t="shared" ref="G45" si="1">IFERROR(F45/C45,)</f>
-        <v>0</v>
-      </c>
-      <c r="H45" s="17"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="14">
-        <f t="shared" ref="J45" si="2">I45-F45</f>
-        <v>0</v>
-      </c>
-      <c r="K45" s="17"/>
-      <c r="L45" s="14" t="str">
-        <f>IF(K45&gt;0,K45*20,"-")</f>
-        <v>-</v>
-      </c>
-      <c r="M45" s="17"/>
-      <c r="N45" s="34"/>
-      <c r="O45" s="14">
-        <f>IFERROR(F45/H45,)</f>
-        <v>0</v>
-      </c>
-      <c r="P45" s="15">
-        <f>IFERROR(H45/C45,)</f>
-        <v>0</v>
-      </c>
-      <c r="Q45" s="14">
-        <f>IFERROR(I45/H45,)</f>
-        <v>0</v>
-      </c>
-      <c r="R45" s="13">
-        <f>IFERROR(I45/F45,)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="2:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="29">
-        <f>IFERROR(C46/D46,)</f>
-        <v>0</v>
-      </c>
-      <c r="F46" s="30"/>
-      <c r="G46" s="31">
-        <f>IFERROR(F46/C46,)</f>
-        <v>0</v>
-      </c>
-      <c r="H46" s="28"/>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30">
-        <f>I46-F46</f>
-        <v>0</v>
-      </c>
-      <c r="K46" s="28"/>
-      <c r="L46" s="30" t="str">
-        <f>IF(K46&gt;0,K46*20,"-")</f>
-        <v>-</v>
-      </c>
-      <c r="M46" s="28"/>
-      <c r="N46" s="35"/>
-      <c r="O46" s="30">
-        <f>IFERROR(F46/H46,)</f>
-        <v>0</v>
-      </c>
-      <c r="P46" s="32">
-        <f>IFERROR(H46/C46,)</f>
-        <v>0</v>
-      </c>
-      <c r="Q46" s="30">
-        <f>IFERROR(I46/H46,)</f>
-        <v>0</v>
-      </c>
-      <c r="R46" s="33">
-        <f>IFERROR(I46/F46,)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="2:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="22">
-        <f>IFERROR(C47/D47,)</f>
-        <v>0</v>
-      </c>
-      <c r="F47" s="23"/>
-      <c r="G47" s="23">
-        <f>IFERROR(F47/C47,)</f>
-        <v>0</v>
-      </c>
-      <c r="H47" s="21"/>
-      <c r="I47" s="24"/>
-      <c r="J47" s="24">
-        <f>I47-F47</f>
-        <v>0</v>
-      </c>
-      <c r="K47" s="21"/>
-      <c r="L47" s="24" t="str">
-        <f>IF(K47&gt;0,K47*20,"-")</f>
-        <v>-</v>
-      </c>
-      <c r="M47" s="21"/>
-      <c r="N47" s="36"/>
-      <c r="O47" s="24">
-        <f>IFERROR(F47/H47,)</f>
-        <v>0</v>
-      </c>
-      <c r="P47" s="25">
-        <f>IFERROR(H47/C47,)</f>
-        <v>0</v>
-      </c>
-      <c r="Q47" s="24">
-        <f>IFERROR(I47/H47,)</f>
-        <v>0</v>
-      </c>
-      <c r="R47" s="26">
-        <f>IFERROR(I47/F47,)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B49" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-      <c r="Q49" s="2"/>
-      <c r="R49" s="2"/>
-      <c r="S49" s="2"/>
-      <c r="T49" s="2"/>
-    </row>
-    <row r="50" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I50" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K50" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L50" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M50" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N50" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O50" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="P50" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q50" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="R50" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="B51" s="18"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="15">
-        <f t="shared" ref="E51" si="3">IFERROR(C51/D51,)</f>
-        <v>0</v>
-      </c>
-      <c r="F51" s="16"/>
-      <c r="G51" s="14">
-        <f t="shared" ref="G51" si="4">IFERROR(F51/C51,)</f>
-        <v>0</v>
-      </c>
-      <c r="H51" s="17"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14">
-        <f t="shared" ref="J51" si="5">I51-F51</f>
-        <v>0</v>
-      </c>
-      <c r="K51" s="17"/>
-      <c r="L51" s="14" t="str">
-        <f>IF(K51&gt;0,K51*20,"-")</f>
-        <v>-</v>
-      </c>
-      <c r="M51" s="17"/>
-      <c r="N51" s="34"/>
-      <c r="O51" s="14">
-        <f>IFERROR(F51/H51,)</f>
-        <v>0</v>
-      </c>
-      <c r="P51" s="15">
-        <f>IFERROR(H51/C51,)</f>
-        <v>0</v>
-      </c>
-      <c r="Q51" s="14">
-        <f>IFERROR(I51/H51,)</f>
-        <v>0</v>
-      </c>
-      <c r="R51" s="13">
-        <f>IFERROR(I51/F51,)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="2:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C52" s="28"/>
-      <c r="D52" s="28"/>
-      <c r="E52" s="29">
-        <f>IFERROR(C52/D52,)</f>
-        <v>0</v>
-      </c>
-      <c r="F52" s="30"/>
-      <c r="G52" s="31">
-        <f>IFERROR(F52/C52,)</f>
-        <v>0</v>
-      </c>
-      <c r="H52" s="28"/>
-      <c r="I52" s="30"/>
-      <c r="J52" s="30">
-        <f>I52-F52</f>
-        <v>0</v>
-      </c>
-      <c r="K52" s="28"/>
-      <c r="L52" s="30" t="str">
+    <row r="52" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="B52" s="18"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="15">
+        <f t="shared" ref="E52" si="0">IFERROR(C52/D52,)</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="16"/>
+      <c r="G52" s="14">
+        <f t="shared" ref="G52" si="1">IFERROR(F52/C52,)</f>
+        <v>0</v>
+      </c>
+      <c r="H52" s="17"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14">
+        <f t="shared" ref="J52" si="2">I52-F52</f>
+        <v>0</v>
+      </c>
+      <c r="K52" s="17"/>
+      <c r="L52" s="14" t="str">
         <f>IF(K52&gt;0,K52*20,"-")</f>
         <v>-</v>
       </c>
-      <c r="M52" s="28"/>
-      <c r="N52" s="35"/>
-      <c r="O52" s="30">
+      <c r="M52" s="17"/>
+      <c r="N52" s="34"/>
+      <c r="O52" s="14">
         <f>IFERROR(F52/H52,)</f>
         <v>0</v>
       </c>
-      <c r="P52" s="32">
+      <c r="P52" s="15">
         <f>IFERROR(H52/C52,)</f>
         <v>0</v>
       </c>
-      <c r="Q52" s="30">
+      <c r="Q52" s="14">
         <f>IFERROR(I52/H52,)</f>
         <v>0</v>
       </c>
-      <c r="R52" s="33">
+      <c r="R52" s="13">
         <f>IFERROR(I52/F52,)</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="2:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
-      <c r="E53" s="22">
+      <c r="B53" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" s="28"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="29">
         <f>IFERROR(C53/D53,)</f>
         <v>0</v>
       </c>
-      <c r="F53" s="23"/>
-      <c r="G53" s="23">
+      <c r="F53" s="30"/>
+      <c r="G53" s="31">
         <f>IFERROR(F53/C53,)</f>
         <v>0</v>
       </c>
-      <c r="H53" s="21"/>
-      <c r="I53" s="24"/>
-      <c r="J53" s="24">
+      <c r="H53" s="28"/>
+      <c r="I53" s="30"/>
+      <c r="J53" s="30">
         <f>I53-F53</f>
         <v>0</v>
       </c>
-      <c r="K53" s="21"/>
-      <c r="L53" s="24" t="str">
+      <c r="K53" s="28"/>
+      <c r="L53" s="30" t="str">
         <f>IF(K53&gt;0,K53*20,"-")</f>
         <v>-</v>
       </c>
-      <c r="M53" s="21"/>
-      <c r="N53" s="36"/>
-      <c r="O53" s="24">
+      <c r="M53" s="28"/>
+      <c r="N53" s="35"/>
+      <c r="O53" s="30">
         <f>IFERROR(F53/H53,)</f>
         <v>0</v>
       </c>
-      <c r="P53" s="25">
+      <c r="P53" s="32">
         <f>IFERROR(H53/C53,)</f>
         <v>0</v>
       </c>
-      <c r="Q53" s="24">
+      <c r="Q53" s="30">
         <f>IFERROR(I53/H53,)</f>
         <v>0</v>
       </c>
-      <c r="R53" s="26">
+      <c r="R53" s="33">
         <f>IFERROR(I53/F53,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="22">
+        <f>IFERROR(C54/D54,)</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="23"/>
+      <c r="G54" s="23">
+        <f>IFERROR(F54/C54,)</f>
+        <v>0</v>
+      </c>
+      <c r="H54" s="21"/>
+      <c r="I54" s="24"/>
+      <c r="J54" s="24">
+        <f>I54-F54</f>
+        <v>0</v>
+      </c>
+      <c r="K54" s="21"/>
+      <c r="L54" s="24" t="str">
+        <f>IF(K54&gt;0,K54*20,"-")</f>
+        <v>-</v>
+      </c>
+      <c r="M54" s="21"/>
+      <c r="N54" s="36"/>
+      <c r="O54" s="24">
+        <f>IFERROR(F54/H54,)</f>
+        <v>0</v>
+      </c>
+      <c r="P54" s="25">
+        <f>IFERROR(H54/C54,)</f>
+        <v>0</v>
+      </c>
+      <c r="Q54" s="24">
+        <f>IFERROR(I54/H54,)</f>
+        <v>0</v>
+      </c>
+      <c r="R54" s="26">
+        <f>IFERROR(I54/F54,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B56" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+      <c r="O56" s="2"/>
+      <c r="P56" s="2"/>
+      <c r="Q56" s="2"/>
+      <c r="R56" s="2"/>
+      <c r="S56" s="2"/>
+      <c r="T56" s="2"/>
+    </row>
+    <row r="57" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K57" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L57" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M57" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N57" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O57" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P57" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q57" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="R57" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="B58" s="18"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="15">
+        <f t="shared" ref="E58" si="3">IFERROR(C58/D58,)</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="16"/>
+      <c r="G58" s="14">
+        <f t="shared" ref="G58" si="4">IFERROR(F58/C58,)</f>
+        <v>0</v>
+      </c>
+      <c r="H58" s="17"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14">
+        <f t="shared" ref="J58" si="5">I58-F58</f>
+        <v>0</v>
+      </c>
+      <c r="K58" s="17"/>
+      <c r="L58" s="14" t="str">
+        <f>IF(K58&gt;0,K58*20,"-")</f>
+        <v>-</v>
+      </c>
+      <c r="M58" s="17"/>
+      <c r="N58" s="34"/>
+      <c r="O58" s="14">
+        <f>IFERROR(F58/H58,)</f>
+        <v>0</v>
+      </c>
+      <c r="P58" s="15">
+        <f>IFERROR(H58/C58,)</f>
+        <v>0</v>
+      </c>
+      <c r="Q58" s="14">
+        <f>IFERROR(I58/H58,)</f>
+        <v>0</v>
+      </c>
+      <c r="R58" s="13">
+        <f>IFERROR(I58/F58,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" s="28"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="29">
+        <f>IFERROR(C59/D59,)</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="30"/>
+      <c r="G59" s="31">
+        <f>IFERROR(F59/C59,)</f>
+        <v>0</v>
+      </c>
+      <c r="H59" s="28"/>
+      <c r="I59" s="30"/>
+      <c r="J59" s="30">
+        <f>I59-F59</f>
+        <v>0</v>
+      </c>
+      <c r="K59" s="28"/>
+      <c r="L59" s="30" t="str">
+        <f>IF(K59&gt;0,K59*20,"-")</f>
+        <v>-</v>
+      </c>
+      <c r="M59" s="28"/>
+      <c r="N59" s="35"/>
+      <c r="O59" s="30">
+        <f>IFERROR(F59/H59,)</f>
+        <v>0</v>
+      </c>
+      <c r="P59" s="32">
+        <f>IFERROR(H59/C59,)</f>
+        <v>0</v>
+      </c>
+      <c r="Q59" s="30">
+        <f>IFERROR(I59/H59,)</f>
+        <v>0</v>
+      </c>
+      <c r="R59" s="33">
+        <f>IFERROR(I59/F59,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="22">
+        <f>IFERROR(C60/D60,)</f>
+        <v>0</v>
+      </c>
+      <c r="F60" s="23"/>
+      <c r="G60" s="23">
+        <f>IFERROR(F60/C60,)</f>
+        <v>0</v>
+      </c>
+      <c r="H60" s="21"/>
+      <c r="I60" s="24"/>
+      <c r="J60" s="24">
+        <f>I60-F60</f>
+        <v>0</v>
+      </c>
+      <c r="K60" s="21"/>
+      <c r="L60" s="24" t="str">
+        <f>IF(K60&gt;0,K60*20,"-")</f>
+        <v>-</v>
+      </c>
+      <c r="M60" s="21"/>
+      <c r="N60" s="36"/>
+      <c r="O60" s="24">
+        <f>IFERROR(F60/H60,)</f>
+        <v>0</v>
+      </c>
+      <c r="P60" s="25">
+        <f>IFERROR(H60/C60,)</f>
+        <v>0</v>
+      </c>
+      <c r="Q60" s="24">
+        <f>IFERROR(I60/H60,)</f>
+        <v>0</v>
+      </c>
+      <c r="R60" s="26">
+        <f>IFERROR(I60/F60,)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B24:N24"/>
-    <mergeCell ref="O24:T24"/>
+    <mergeCell ref="B31:N31"/>
+    <mergeCell ref="O31:T31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Search Portal WoW: remove blank row above WoW section, add borders
</commit_message>
<xml_diff>
--- a/3/DAGenerators/Spreadsheets/Templates/search/SearchPPCtemplate.xlsx
+++ b/3/DAGenerators/Spreadsheets/Templates/search/SearchPPCtemplate.xlsx
@@ -327,7 +327,7 @@
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -445,6 +445,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -803,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B8:T60"/>
+  <dimension ref="B8:T59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+      <selection activeCell="B30" sqref="B30:N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,25 +1276,25 @@
       </c>
     </row>
     <row r="22" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="44"/>
+      <c r="P22" s="44"/>
+      <c r="Q22" s="44"/>
+      <c r="R22" s="44"/>
     </row>
     <row r="23" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
@@ -1309,97 +1315,123 @@
       <c r="Q23" s="15"/>
       <c r="R23" s="15"/>
     </row>
-    <row r="24" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="13"/>
-    </row>
-    <row r="25" spans="2:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="10" t="s">
+    <row r="24" spans="2:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-    </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="4" t="s">
+      <c r="C25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H25" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="I25" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="J25" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K26" s="4" t="s">
+      <c r="K25" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L26" s="4" t="s">
+      <c r="L25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M26" s="4" t="s">
+      <c r="M25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="N26" s="4" t="s">
+      <c r="N25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="O26" s="4" t="s">
+      <c r="O25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P26" s="6" t="s">
+      <c r="P25" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q26" s="4" t="s">
+      <c r="Q25" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="R26" s="6" t="s">
+      <c r="R25" s="6" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="15">
+        <f>IFERROR(C26/D26,)</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="16"/>
+      <c r="G26" s="14">
+        <f>IFERROR(F26/C26,)</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="17"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14">
+        <f>I26-F26</f>
+        <v>0</v>
+      </c>
+      <c r="K26" s="17"/>
+      <c r="L26" s="14" t="str">
+        <f>IF(K26&gt;0,K26*20,"-")</f>
+        <v>-</v>
+      </c>
+      <c r="M26" s="17"/>
+      <c r="N26" s="34"/>
+      <c r="O26" s="14">
+        <f>IFERROR(F26/H26,)</f>
+        <v>0</v>
+      </c>
+      <c r="P26" s="15">
+        <f>IFERROR(H26/C26,)</f>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="14">
+        <f>IFERROR(I26/H26,)</f>
+        <v>0</v>
+      </c>
+      <c r="R26" s="13">
+        <f>IFERROR(I26/F26,)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
@@ -1446,536 +1478,493 @@
       </c>
     </row>
     <row r="28" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="15">
-        <f>IFERROR(C28/D28,)</f>
-        <v>0</v>
-      </c>
-      <c r="F28" s="16"/>
-      <c r="G28" s="14">
-        <f>IFERROR(F28/C28,)</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="17"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14">
-        <f>I28-F28</f>
-        <v>0</v>
-      </c>
-      <c r="K28" s="17"/>
-      <c r="L28" s="14" t="str">
-        <f>IF(K28&gt;0,K28*20,"-")</f>
+      <c r="B28" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="44"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="44"/>
+      <c r="O28" s="44"/>
+      <c r="P28" s="44"/>
+      <c r="Q28" s="44"/>
+      <c r="R28" s="44"/>
+    </row>
+    <row r="29" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="B29" s="7"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="14"/>
+      <c r="P29" s="13"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="45"/>
+      <c r="M30" s="45"/>
+      <c r="N30" s="45"/>
+      <c r="O30" s="45"/>
+      <c r="P30" s="45"/>
+      <c r="Q30" s="45"/>
+      <c r="R30" s="45"/>
+      <c r="S30" s="45"/>
+      <c r="T30" s="45"/>
+    </row>
+    <row r="34" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O34" s="8"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
+    </row>
+    <row r="49" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B49" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="2"/>
+      <c r="S49" s="2"/>
+      <c r="T49" s="2"/>
+    </row>
+    <row r="50" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L50" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N50" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O50" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P50" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q50" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="R50" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="B51" s="18"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="15">
+        <f t="shared" ref="E51" si="0">IFERROR(C51/D51,)</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="16"/>
+      <c r="G51" s="14">
+        <f t="shared" ref="G51" si="1">IFERROR(F51/C51,)</f>
+        <v>0</v>
+      </c>
+      <c r="H51" s="17"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14">
+        <f t="shared" ref="J51" si="2">I51-F51</f>
+        <v>0</v>
+      </c>
+      <c r="K51" s="17"/>
+      <c r="L51" s="14" t="str">
+        <f>IF(K51&gt;0,K51*20,"-")</f>
         <v>-</v>
       </c>
-      <c r="M28" s="17"/>
-      <c r="N28" s="34"/>
-      <c r="O28" s="14">
-        <f>IFERROR(F28/H28,)</f>
-        <v>0</v>
-      </c>
-      <c r="P28" s="15">
-        <f>IFERROR(H28/C28,)</f>
-        <v>0</v>
-      </c>
-      <c r="Q28" s="14">
-        <f>IFERROR(I28/H28,)</f>
-        <v>0</v>
-      </c>
-      <c r="R28" s="13">
-        <f>IFERROR(I28/F28,)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="B29" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
-    </row>
-    <row r="30" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="13"/>
-    </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B31" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="43"/>
-      <c r="M31" s="43"/>
-      <c r="N31" s="43"/>
-      <c r="O31" s="43"/>
-      <c r="P31" s="43"/>
-      <c r="Q31" s="43"/>
-      <c r="R31" s="43"/>
-      <c r="S31" s="43"/>
-      <c r="T31" s="43"/>
-    </row>
-    <row r="35" spans="15:17" x14ac:dyDescent="0.25">
-      <c r="O35" s="8"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="9"/>
-    </row>
-    <row r="50" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B50" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
-      <c r="O50" s="2"/>
-      <c r="P50" s="2"/>
-      <c r="Q50" s="2"/>
-      <c r="R50" s="2"/>
-      <c r="S50" s="2"/>
-      <c r="T50" s="2"/>
-    </row>
-    <row r="51" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J51" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K51" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L51" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M51" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N51" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O51" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="P51" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q51" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="R51" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="B52" s="18"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="15">
-        <f t="shared" ref="E52" si="0">IFERROR(C52/D52,)</f>
-        <v>0</v>
-      </c>
-      <c r="F52" s="16"/>
-      <c r="G52" s="14">
-        <f t="shared" ref="G52" si="1">IFERROR(F52/C52,)</f>
-        <v>0</v>
-      </c>
-      <c r="H52" s="17"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14">
-        <f t="shared" ref="J52" si="2">I52-F52</f>
-        <v>0</v>
-      </c>
-      <c r="K52" s="17"/>
-      <c r="L52" s="14" t="str">
+      <c r="M51" s="17"/>
+      <c r="N51" s="34"/>
+      <c r="O51" s="14">
+        <f>IFERROR(F51/H51,)</f>
+        <v>0</v>
+      </c>
+      <c r="P51" s="15">
+        <f>IFERROR(H51/C51,)</f>
+        <v>0</v>
+      </c>
+      <c r="Q51" s="14">
+        <f>IFERROR(I51/H51,)</f>
+        <v>0</v>
+      </c>
+      <c r="R51" s="13">
+        <f>IFERROR(I51/F51,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="29">
+        <f>IFERROR(C52/D52,)</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="30"/>
+      <c r="G52" s="31">
+        <f>IFERROR(F52/C52,)</f>
+        <v>0</v>
+      </c>
+      <c r="H52" s="28"/>
+      <c r="I52" s="30"/>
+      <c r="J52" s="30">
+        <f>I52-F52</f>
+        <v>0</v>
+      </c>
+      <c r="K52" s="28"/>
+      <c r="L52" s="30" t="str">
         <f>IF(K52&gt;0,K52*20,"-")</f>
         <v>-</v>
       </c>
-      <c r="M52" s="17"/>
-      <c r="N52" s="34"/>
-      <c r="O52" s="14">
+      <c r="M52" s="28"/>
+      <c r="N52" s="35"/>
+      <c r="O52" s="30">
         <f>IFERROR(F52/H52,)</f>
         <v>0</v>
       </c>
-      <c r="P52" s="15">
+      <c r="P52" s="32">
         <f>IFERROR(H52/C52,)</f>
         <v>0</v>
       </c>
-      <c r="Q52" s="14">
+      <c r="Q52" s="30">
         <f>IFERROR(I52/H52,)</f>
         <v>0</v>
       </c>
-      <c r="R52" s="13">
+      <c r="R52" s="33">
         <f>IFERROR(I52/F52,)</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="2:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="29">
+      <c r="B53" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="22">
         <f>IFERROR(C53/D53,)</f>
         <v>0</v>
       </c>
-      <c r="F53" s="30"/>
-      <c r="G53" s="31">
+      <c r="F53" s="23"/>
+      <c r="G53" s="23">
         <f>IFERROR(F53/C53,)</f>
         <v>0</v>
       </c>
-      <c r="H53" s="28"/>
-      <c r="I53" s="30"/>
-      <c r="J53" s="30">
+      <c r="H53" s="21"/>
+      <c r="I53" s="24"/>
+      <c r="J53" s="24">
         <f>I53-F53</f>
         <v>0</v>
       </c>
-      <c r="K53" s="28"/>
-      <c r="L53" s="30" t="str">
+      <c r="K53" s="21"/>
+      <c r="L53" s="24" t="str">
         <f>IF(K53&gt;0,K53*20,"-")</f>
         <v>-</v>
       </c>
-      <c r="M53" s="28"/>
-      <c r="N53" s="35"/>
-      <c r="O53" s="30">
+      <c r="M53" s="21"/>
+      <c r="N53" s="36"/>
+      <c r="O53" s="24">
         <f>IFERROR(F53/H53,)</f>
         <v>0</v>
       </c>
-      <c r="P53" s="32">
+      <c r="P53" s="25">
         <f>IFERROR(H53/C53,)</f>
         <v>0</v>
       </c>
-      <c r="Q53" s="30">
+      <c r="Q53" s="24">
         <f>IFERROR(I53/H53,)</f>
         <v>0</v>
       </c>
-      <c r="R53" s="33">
+      <c r="R53" s="26">
         <f>IFERROR(I53/F53,)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
-      <c r="E54" s="22">
-        <f>IFERROR(C54/D54,)</f>
-        <v>0</v>
-      </c>
-      <c r="F54" s="23"/>
-      <c r="G54" s="23">
-        <f>IFERROR(F54/C54,)</f>
-        <v>0</v>
-      </c>
-      <c r="H54" s="21"/>
-      <c r="I54" s="24"/>
-      <c r="J54" s="24">
-        <f>I54-F54</f>
-        <v>0</v>
-      </c>
-      <c r="K54" s="21"/>
-      <c r="L54" s="24" t="str">
-        <f>IF(K54&gt;0,K54*20,"-")</f>
+    <row r="55" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B55" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="2"/>
+      <c r="R55" s="2"/>
+      <c r="S55" s="2"/>
+      <c r="T55" s="2"/>
+    </row>
+    <row r="56" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K56" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L56" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M56" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N56" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O56" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P56" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q56" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="R56" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="B57" s="18"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="15">
+        <f t="shared" ref="E57" si="3">IFERROR(C57/D57,)</f>
+        <v>0</v>
+      </c>
+      <c r="F57" s="16"/>
+      <c r="G57" s="14">
+        <f t="shared" ref="G57" si="4">IFERROR(F57/C57,)</f>
+        <v>0</v>
+      </c>
+      <c r="H57" s="17"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14">
+        <f t="shared" ref="J57" si="5">I57-F57</f>
+        <v>0</v>
+      </c>
+      <c r="K57" s="17"/>
+      <c r="L57" s="14" t="str">
+        <f>IF(K57&gt;0,K57*20,"-")</f>
         <v>-</v>
       </c>
-      <c r="M54" s="21"/>
-      <c r="N54" s="36"/>
-      <c r="O54" s="24">
-        <f>IFERROR(F54/H54,)</f>
-        <v>0</v>
-      </c>
-      <c r="P54" s="25">
-        <f>IFERROR(H54/C54,)</f>
-        <v>0</v>
-      </c>
-      <c r="Q54" s="24">
-        <f>IFERROR(I54/H54,)</f>
-        <v>0</v>
-      </c>
-      <c r="R54" s="26">
-        <f>IFERROR(I54/F54,)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B56" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
-      <c r="L56" s="2"/>
-      <c r="M56" s="2"/>
-      <c r="N56" s="2"/>
-      <c r="O56" s="2"/>
-      <c r="P56" s="2"/>
-      <c r="Q56" s="2"/>
-      <c r="R56" s="2"/>
-      <c r="S56" s="2"/>
-      <c r="T56" s="2"/>
-    </row>
-    <row r="57" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I57" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J57" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K57" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L57" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M57" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N57" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O57" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="P57" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q57" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="R57" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="2:20" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="B58" s="18"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="15">
-        <f t="shared" ref="E58" si="3">IFERROR(C58/D58,)</f>
-        <v>0</v>
-      </c>
-      <c r="F58" s="16"/>
-      <c r="G58" s="14">
-        <f t="shared" ref="G58" si="4">IFERROR(F58/C58,)</f>
-        <v>0</v>
-      </c>
-      <c r="H58" s="17"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="14">
-        <f t="shared" ref="J58" si="5">I58-F58</f>
-        <v>0</v>
-      </c>
-      <c r="K58" s="17"/>
-      <c r="L58" s="14" t="str">
+      <c r="M57" s="17"/>
+      <c r="N57" s="34"/>
+      <c r="O57" s="14">
+        <f>IFERROR(F57/H57,)</f>
+        <v>0</v>
+      </c>
+      <c r="P57" s="15">
+        <f>IFERROR(H57/C57,)</f>
+        <v>0</v>
+      </c>
+      <c r="Q57" s="14">
+        <f>IFERROR(I57/H57,)</f>
+        <v>0</v>
+      </c>
+      <c r="R57" s="13">
+        <f>IFERROR(I57/F57,)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C58" s="28"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="29">
+        <f>IFERROR(C58/D58,)</f>
+        <v>0</v>
+      </c>
+      <c r="F58" s="30"/>
+      <c r="G58" s="31">
+        <f>IFERROR(F58/C58,)</f>
+        <v>0</v>
+      </c>
+      <c r="H58" s="28"/>
+      <c r="I58" s="30"/>
+      <c r="J58" s="30">
+        <f>I58-F58</f>
+        <v>0</v>
+      </c>
+      <c r="K58" s="28"/>
+      <c r="L58" s="30" t="str">
         <f>IF(K58&gt;0,K58*20,"-")</f>
         <v>-</v>
       </c>
-      <c r="M58" s="17"/>
-      <c r="N58" s="34"/>
-      <c r="O58" s="14">
+      <c r="M58" s="28"/>
+      <c r="N58" s="35"/>
+      <c r="O58" s="30">
         <f>IFERROR(F58/H58,)</f>
         <v>0</v>
       </c>
-      <c r="P58" s="15">
+      <c r="P58" s="32">
         <f>IFERROR(H58/C58,)</f>
         <v>0</v>
       </c>
-      <c r="Q58" s="14">
+      <c r="Q58" s="30">
         <f>IFERROR(I58/H58,)</f>
         <v>0</v>
       </c>
-      <c r="R58" s="13">
+      <c r="R58" s="33">
         <f>IFERROR(I58/F58,)</f>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="2:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C59" s="28"/>
-      <c r="D59" s="28"/>
-      <c r="E59" s="29">
+      <c r="B59" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="22">
         <f>IFERROR(C59/D59,)</f>
         <v>0</v>
       </c>
-      <c r="F59" s="30"/>
-      <c r="G59" s="31">
+      <c r="F59" s="23"/>
+      <c r="G59" s="23">
         <f>IFERROR(F59/C59,)</f>
         <v>0</v>
       </c>
-      <c r="H59" s="28"/>
-      <c r="I59" s="30"/>
-      <c r="J59" s="30">
+      <c r="H59" s="21"/>
+      <c r="I59" s="24"/>
+      <c r="J59" s="24">
         <f>I59-F59</f>
         <v>0</v>
       </c>
-      <c r="K59" s="28"/>
-      <c r="L59" s="30" t="str">
+      <c r="K59" s="21"/>
+      <c r="L59" s="24" t="str">
         <f>IF(K59&gt;0,K59*20,"-")</f>
         <v>-</v>
       </c>
-      <c r="M59" s="28"/>
-      <c r="N59" s="35"/>
-      <c r="O59" s="30">
+      <c r="M59" s="21"/>
+      <c r="N59" s="36"/>
+      <c r="O59" s="24">
         <f>IFERROR(F59/H59,)</f>
         <v>0</v>
       </c>
-      <c r="P59" s="32">
+      <c r="P59" s="25">
         <f>IFERROR(H59/C59,)</f>
         <v>0</v>
       </c>
-      <c r="Q59" s="30">
+      <c r="Q59" s="24">
         <f>IFERROR(I59/H59,)</f>
         <v>0</v>
       </c>
-      <c r="R59" s="33">
+      <c r="R59" s="26">
         <f>IFERROR(I59/F59,)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="2:20" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C60" s="21"/>
-      <c r="D60" s="21"/>
-      <c r="E60" s="22">
-        <f>IFERROR(C60/D60,)</f>
-        <v>0</v>
-      </c>
-      <c r="F60" s="23"/>
-      <c r="G60" s="23">
-        <f>IFERROR(F60/C60,)</f>
-        <v>0</v>
-      </c>
-      <c r="H60" s="21"/>
-      <c r="I60" s="24"/>
-      <c r="J60" s="24">
-        <f>I60-F60</f>
-        <v>0</v>
-      </c>
-      <c r="K60" s="21"/>
-      <c r="L60" s="24" t="str">
-        <f>IF(K60&gt;0,K60*20,"-")</f>
-        <v>-</v>
-      </c>
-      <c r="M60" s="21"/>
-      <c r="N60" s="36"/>
-      <c r="O60" s="24">
-        <f>IFERROR(F60/H60,)</f>
-        <v>0</v>
-      </c>
-      <c r="P60" s="25">
-        <f>IFERROR(H60/C60,)</f>
-        <v>0</v>
-      </c>
-      <c r="Q60" s="24">
-        <f>IFERROR(I60/H60,)</f>
-        <v>0</v>
-      </c>
-      <c r="R60" s="26">
-        <f>IFERROR(I60/F60,)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B31:N31"/>
-    <mergeCell ref="O31:T31"/>
+    <mergeCell ref="B30:N30"/>
+    <mergeCell ref="O30:T30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
new logos for search reports, misc
</commit_message>
<xml_diff>
--- a/3/DAGenerators/Spreadsheets/Templates/search/SearchPPCtemplate.xlsx
+++ b/3/DAGenerators/Spreadsheets/Templates/search/SearchPPCtemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\da-projects\3\DAGenerators\Spreadsheets\Templates\search\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DA\portal\search\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -482,13 +482,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>95082</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>198307</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>39733</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>163725</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -496,7 +496,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -509,8 +509,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="581025" y="219075"/>
-          <a:ext cx="7313482" cy="963658"/>
+          <a:off x="581025" y="285582"/>
+          <a:ext cx="7313482" cy="830643"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -811,9 +811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B8:T59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:N30"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1977,7 +1975,7 @@
   <dimension ref="B10:T12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2088,7 +2086,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T8"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>